<commit_message>
initial localisation system rev
</commit_message>
<xml_diff>
--- a/docs/v0.1.0.xlsx
+++ b/docs/v0.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7035536A-8599-4BE3-866B-63F13A61D93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC852462-2AB1-4C10-A49F-CCCFBC4F5BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3B64DF0-D13F-44EC-B65D-E8C09BC72989}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>Task</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>Write Font Engine documentation</t>
+  </si>
+  <si>
+    <t>Write Localisation documentation</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -209,12 +215,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -229,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -238,6 +250,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2698D1-E58C-4BD1-883E-F12402E4C873}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -787,6 +800,12 @@
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C26" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="2">
+        <v>45473</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -821,75 +840,83 @@
         <v>29</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" s="1" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix arrow keys in legacy UI
</commit_message>
<xml_diff>
--- a/docs/v0.1.0.xlsx
+++ b/docs/v0.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC852462-2AB1-4C10-A49F-CCCFBC4F5BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33539C0E-B07B-44E4-8217-CC7152E70FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3B64DF0-D13F-44EC-B65D-E8C09BC72989}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Task</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Account system incl. Premium</t>
   </si>
   <si>
-    <t>Top down???</t>
-  </si>
-  <si>
     <t>Account, IP ban</t>
   </si>
   <si>
@@ -187,6 +184,15 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Fix: Can never reenter a server if you quit with TeamUI active</t>
+  </si>
+  <si>
+    <t>BbUGFIX</t>
+  </si>
+  <si>
+    <t>Top down camera and camera rewrite</t>
   </si>
 </sst>
 </file>
@@ -567,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2698D1-E58C-4BD1-883E-F12402E4C873}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A18" sqref="A3:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -704,74 +710,74 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="2"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>17</v>
@@ -779,15 +785,18 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C24" s="6" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
@@ -795,29 +804,29 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="2">
-        <v>45473</v>
-      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="2">
+        <v>45473</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>17</v>
@@ -825,24 +834,24 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="3"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>29</v>
@@ -850,7 +859,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>29</v>
@@ -858,7 +867,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>29</v>
@@ -866,7 +875,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>29</v>
@@ -874,7 +883,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>29</v>
@@ -882,7 +891,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>29</v>
@@ -890,7 +899,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>29</v>
@@ -898,26 +907,34 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working alternative camera angles, prediction needs to be rewritten etc
</commit_message>
<xml_diff>
--- a/docs/v0.1.0.xlsx
+++ b/docs/v0.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33539C0E-B07B-44E4-8217-CC7152E70FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F8C9CA-B484-4475-8D9F-56DCE0006419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3B64DF0-D13F-44EC-B65D-E8C09BC72989}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>Task</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Add kill feed</t>
   </si>
   <si>
-    <t>z_tdm_warehouse - Second Floor</t>
-  </si>
-  <si>
     <t>Make Master servers work</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>Allow people to see what team a player is</t>
   </si>
   <si>
-    <t>Real updater</t>
-  </si>
-  <si>
     <t>z_waves_port working (THEY COME FROM THE SEA/!?!?!?!?!) - z_tdm_spire finished</t>
   </si>
   <si>
@@ -189,10 +183,16 @@
     <t>Fix: Can never reenter a server if you quit with TeamUI active</t>
   </si>
   <si>
-    <t>BbUGFIX</t>
-  </si>
-  <si>
     <t>Top down camera and camera rewrite</t>
+  </si>
+  <si>
+    <t>z_tdm_warehouse - Redesign</t>
+  </si>
+  <si>
+    <t>Real updater (hash based)</t>
+  </si>
+  <si>
+    <t>Fix: Legacy UI arrow keys</t>
   </si>
 </sst>
 </file>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2698D1-E58C-4BD1-883E-F12402E4C873}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A18" sqref="A3:B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -588,10 +588,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -634,7 +634,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
@@ -710,101 +710,116 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2">
+        <v>45491</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45473</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21" s="2"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C25" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="2">
+        <v>45483</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>17</v>
@@ -812,29 +827,29 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D27" s="2">
-        <v>45473</v>
-      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C28" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="2">
+        <v>45473</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>17</v>
@@ -842,104 +857,112 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="3"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
that was completedly incorrect, we actually just failed to send any movement commands if a ui was active, make sure the client is connected instad of doing that
</commit_message>
<xml_diff>
--- a/docs/v0.1.0.xlsx
+++ b/docs/v0.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F8C9CA-B484-4475-8D9F-56DCE0006419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0598F3-5D92-47E8-ADEE-1DA103E076B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3B64DF0-D13F-44EC-B65D-E8C09BC72989}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>Task</t>
   </si>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2698D1-E58C-4BD1-883E-F12402E4C873}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -715,6 +715,9 @@
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C15" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -861,6 +864,12 @@
       </c>
       <c r="B30" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="2">
+        <v>45497</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
implement CPUID subsystem and rewrite localisation key loading to be a lot more sane
</commit_message>
<xml_diff>
--- a/docs/v0.1.0.xlsx
+++ b/docs/v0.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0598F3-5D92-47E8-ADEE-1DA103E076B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D59A6A-0BBA-4BC6-9191-668F94E30C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3B64DF0-D13F-44EC-B65D-E8C09BC72989}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>Task</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Fix: Legacy UI arrow keys</t>
+  </si>
+  <si>
+    <t>Fix: line -&gt; comment -&gt; line leads to skip in localisation parser?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix: Only one localisation key reference works in localisation string </t>
   </si>
 </sst>
 </file>
@@ -573,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2698D1-E58C-4BD1-883E-F12402E4C873}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -735,94 +741,88 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="2">
-        <v>45473</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="2">
+        <v>45473</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="2"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="2">
-        <v>45483</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>17</v>
@@ -830,29 +830,29 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C27" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="2">
+        <v>45483</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="2">
-        <v>45473</v>
-      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>17</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>17</v>
@@ -869,103 +869,125 @@
         <v>50</v>
       </c>
       <c r="D30" s="2">
-        <v>45497</v>
+        <v>45473</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="2">
+        <v>45497</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
initial revision of killfeed, add the ability to set ui position and size after adding the ui
</commit_message>
<xml_diff>
--- a/docs/v0.1.0.xlsx
+++ b/docs/v0.1.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D59A6A-0BBA-4BC6-9191-668F94E30C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D300DCE5-108B-4083-802D-EE6B337DAC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3B64DF0-D13F-44EC-B65D-E8C09BC72989}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
   <si>
     <t>Task</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t xml:space="preserve">Fix: Only one localisation key reference works in localisation string </t>
+  </si>
+  <si>
+    <t>Add HTTP POST to Netservices</t>
+  </si>
+  <si>
+    <t>Fix: input</t>
   </si>
 </sst>
 </file>
@@ -579,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B2698D1-E58C-4BD1-883E-F12402E4C873}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -757,94 +763,94 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="2">
-        <v>45473</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="2">
+        <v>45473</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="2"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="2">
+        <v>45509</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="2">
-        <v>45483</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>17</v>
@@ -852,29 +858,29 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="2">
+        <v>45483</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="2">
-        <v>45473</v>
-      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>17</v>
@@ -882,7 +888,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>17</v>
@@ -891,37 +897,43 @@
         <v>50</v>
       </c>
       <c r="D32" s="2">
-        <v>45497</v>
+        <v>45473</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="3"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="2">
+        <v>45497</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>27</v>
@@ -929,7 +941,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>27</v>
@@ -937,7 +949,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>27</v>
@@ -945,7 +957,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>27</v>
@@ -953,7 +965,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>27</v>
@@ -961,7 +973,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>27</v>
@@ -969,25 +981,41 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>